<commit_message>
penultimate doc commit still awaiting some analysis docs
</commit_message>
<xml_diff>
--- a/Documentation/AgileReleaseSummary.xlsx
+++ b/Documentation/AgileReleaseSummary.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
   <si>
     <t>Team:</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Project Plan</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -253,7 +256,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,10 +564,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,7 +672,13 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
@@ -725,7 +734,7 @@
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
     </row>
-    <row r="17" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>8</v>
       </c>
@@ -740,7 +749,7 @@
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
     </row>
-    <row r="18" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>9</v>
       </c>
@@ -755,7 +764,7 @@
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
     </row>
-    <row r="19" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>10</v>
       </c>
@@ -770,7 +779,7 @@
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
     </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>11</v>
       </c>
@@ -785,7 +794,7 @@
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>12</v>
       </c>
@@ -800,7 +809,7 @@
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
     </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>13</v>
       </c>
@@ -815,7 +824,7 @@
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
     </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>14</v>
       </c>
@@ -830,7 +839,7 @@
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>15</v>
       </c>
@@ -845,7 +854,7 @@
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
     </row>
-    <row r="25" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>16</v>
       </c>
@@ -860,7 +869,7 @@
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>17</v>
       </c>
@@ -875,7 +884,7 @@
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
     </row>
-    <row r="27" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>18</v>
       </c>
@@ -890,13 +899,16 @@
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="15"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>19</v>
       </c>
@@ -906,8 +918,11 @@
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
-    </row>
-    <row r="30" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>20</v>
       </c>
@@ -919,8 +934,11 @@
       <c r="E30" s="8"/>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
-    </row>
-    <row r="31" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H30" s="17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>21</v>
       </c>
@@ -932,8 +950,11 @@
       <c r="E31" s="8"/>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
-    </row>
-    <row r="32" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H31" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>22</v>
       </c>
@@ -945,6 +966,9 @@
       <c r="E32" s="8"/>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
+      <c r="H32" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="33" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
@@ -958,6 +982,9 @@
       <c r="E33" s="8"/>
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
+      <c r="H33" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="34" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
@@ -971,6 +998,9 @@
       <c r="E34" s="8"/>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
+      <c r="H34" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="35" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
@@ -984,6 +1014,9 @@
       <c r="E35" s="8"/>
       <c r="F35" s="14"/>
       <c r="G35" s="14"/>
+      <c r="H35" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
@@ -997,6 +1030,9 @@
       <c r="E36" s="8"/>
       <c r="F36" s="14"/>
       <c r="G36" s="14"/>
+      <c r="H36" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
@@ -1010,6 +1046,9 @@
       <c r="E37" s="8"/>
       <c r="F37" s="14"/>
       <c r="G37" s="14"/>
+      <c r="H37" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="38" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
@@ -1023,6 +1062,9 @@
       <c r="E38" s="8"/>
       <c r="F38" s="14"/>
       <c r="G38" s="14"/>
+      <c r="H38" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="39" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
@@ -1033,9 +1075,14 @@
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
+      <c r="E39" s="8">
+        <v>1.5</v>
+      </c>
       <c r="F39" s="14"/>
       <c r="G39" s="14"/>
+      <c r="H39" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="40" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
@@ -1046,9 +1093,14 @@
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
+      <c r="E40" s="8">
+        <v>5</v>
+      </c>
       <c r="F40" s="14"/>
       <c r="G40" s="14"/>
+      <c r="H40" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
@@ -1060,6 +1112,9 @@
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
+      <c r="H41" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
@@ -1071,6 +1126,9 @@
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
+      <c r="H42" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
@@ -1083,69 +1141,61 @@
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
       <c r="F43" s="16"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="8">
-        <v>34</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-    </row>
-    <row r="45" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="16"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
+      <c r="H43" s="17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="15"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="13"/>
+      <c r="B45" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
-      <c r="B46" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
+      <c r="A46" s="14"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="15"/>
-      <c r="B48" s="10" t="s">
+      <c r="A47" s="15"/>
+      <c r="B47" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="15">
+      <c r="C47" s="15">
         <f>SUM(C9:C11)</f>
         <v>14</v>
       </c>
-      <c r="D48" s="15">
+      <c r="D47" s="15">
         <f>SUM(D13:D27)</f>
         <v>58</v>
       </c>
-      <c r="E48" s="15">
-        <f>SUM(E9:E47)</f>
+      <c r="E47" s="15">
+        <f>SUM(E29:E43)</f>
+        <v>6.5</v>
+      </c>
+      <c r="F47" s="15">
+        <f>SUM(F9:F46)</f>
         <v>0</v>
       </c>
-      <c r="F48" s="15">
-        <f>SUM(F9:F47)</f>
+      <c r="G47" s="15">
+        <f>SUM(G9:G46)</f>
         <v>0</v>
       </c>
-      <c r="G48" s="15">
-        <f>SUM(G9:G47)</f>
-        <v>0</v>
-      </c>
-      <c r="H48" s="11">
-        <f>SUM(C48:G48)</f>
-        <v>72</v>
+      <c r="H47" s="11">
+        <f>SUM(C47:G47)</f>
+        <v>78.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final commit from Jeff for this iteration
</commit_message>
<xml_diff>
--- a/Documentation/AgileReleaseSummary.xlsx
+++ b/Documentation/AgileReleaseSummary.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>Team:</t>
   </si>
@@ -129,9 +129,6 @@
   </si>
   <si>
     <t>Project Plan</t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
 </sst>
 </file>
@@ -566,8 +563,8 @@
   </sheetPr>
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,9 +914,8 @@
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="H29" t="s">
-        <v>36</v>
+      <c r="E29" s="8">
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -931,12 +927,12 @@
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
+      <c r="E30" s="8">
+        <v>6</v>
+      </c>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
-      <c r="H30" s="17">
-        <v>0.5</v>
-      </c>
+      <c r="H30" s="17"/>
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
@@ -947,12 +943,11 @@
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
+      <c r="E31" s="8">
+        <v>1.5</v>
+      </c>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
-      <c r="H31" s="1" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="32" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
@@ -963,12 +958,11 @@
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
+      <c r="E32" s="8">
+        <v>2.5</v>
+      </c>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
-      <c r="H32" s="1" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="33" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
@@ -979,12 +973,11 @@
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
+      <c r="E33" s="8">
+        <v>2</v>
+      </c>
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
-      <c r="H33" s="1" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="34" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
@@ -995,12 +988,11 @@
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
+      <c r="E34" s="8">
+        <v>2</v>
+      </c>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
-      <c r="H34" s="1" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="35" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
@@ -1011,12 +1003,12 @@
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
+      <c r="E35" s="8">
+        <v>2</v>
+      </c>
       <c r="F35" s="14"/>
       <c r="G35" s="14"/>
-      <c r="H35" s="17">
-        <v>0</v>
-      </c>
+      <c r="H35" s="17"/>
     </row>
     <row r="36" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
@@ -1027,12 +1019,12 @@
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
+      <c r="E36" s="8">
+        <v>4</v>
+      </c>
       <c r="F36" s="14"/>
       <c r="G36" s="14"/>
-      <c r="H36" s="17">
-        <v>0</v>
-      </c>
+      <c r="H36" s="17"/>
     </row>
     <row r="37" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
@@ -1043,12 +1035,11 @@
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
+      <c r="E37" s="8">
+        <v>3</v>
+      </c>
       <c r="F37" s="14"/>
       <c r="G37" s="14"/>
-      <c r="H37" s="1" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="38" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
@@ -1059,12 +1050,11 @@
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
+      <c r="E38" s="8">
+        <v>2</v>
+      </c>
       <c r="F38" s="14"/>
       <c r="G38" s="14"/>
-      <c r="H38" s="1" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="39" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
@@ -1076,13 +1066,10 @@
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="F39" s="14"/>
       <c r="G39" s="14"/>
-      <c r="H39" s="1" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="40" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
@@ -1098,9 +1085,6 @@
       </c>
       <c r="F40" s="14"/>
       <c r="G40" s="14"/>
-      <c r="H40" s="1" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
@@ -1111,9 +1095,8 @@
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="H41" t="s">
-        <v>36</v>
+      <c r="E41" s="8">
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1125,9 +1108,8 @@
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="H42" t="s">
-        <v>36</v>
+      <c r="E42" s="8">
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -1139,11 +1121,11 @@
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
+      <c r="E43" s="8">
+        <v>3</v>
+      </c>
       <c r="F43" s="16"/>
-      <c r="H43" s="17">
-        <v>0.5</v>
-      </c>
+      <c r="H43" s="17"/>
     </row>
     <row r="44" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="15"/>
@@ -1183,7 +1165,7 @@
       </c>
       <c r="E47" s="15">
         <f>SUM(E29:E43)</f>
-        <v>6.5</v>
+        <v>73</v>
       </c>
       <c r="F47" s="15">
         <f>SUM(F9:F46)</f>
@@ -1195,7 +1177,7 @@
       </c>
       <c r="H47" s="11">
         <f>SUM(C47:G47)</f>
-        <v>78.5</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>